<commit_message>
Update Leave Card 2/16/2024 8:10 AM
</commit_message>
<xml_diff>
--- a/CASUAL/ESTOQUE, AILEEN.xlsx
+++ b/CASUAL/ESTOQUE, AILEEN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DOLE-PC\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818AC11-AC0E-413A-BBBA-464A745F5443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457E1BFD-5B89-4066-979E-EDB40C3347DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>PERIOD</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>ONT</t>
+  </si>
+  <si>
+    <t>SP(1-0-0)</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,6 +554,9 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -587,7 +593,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2958,9 +2964,9 @@
   <dimension ref="A2:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A7"/>
-      <selection activeCell="F5" sqref="F5"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="3576" topLeftCell="A4" activePane="bottomLeft"/>
+      <selection activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2982,64 +2988,64 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="58">
         <v>45154</v>
       </c>
-      <c r="G3" s="54"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="54"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -3065,18 +3071,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3139,7 +3145,7 @@
       <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="20"/>
@@ -3181,8 +3187,12 @@
       <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="40">
+        <v>45351</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="39"/>
       <c r="E12" s="9"/>
@@ -3194,7 +3204,9 @@
       <c r="H12" s="39"/>
       <c r="I12" s="9"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="20"/>
+      <c r="K12" s="61">
+        <v>45350</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40"/>
@@ -5148,17 +5160,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="J1" s="59" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="J1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -5244,12 +5256,12 @@
         <v>30</v>
       </c>
       <c r="G6" s="44"/>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="9">

</xml_diff>